<commit_message>
commiting 1st normal form dataset
</commit_message>
<xml_diff>
--- a/Denormalized Dataset.xlsx
+++ b/Denormalized Dataset.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MySQL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karth\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C72156B9-1CDF-4423-8F10-77FBD824806D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA896BE-B802-4A3B-A3F9-4D584BF00C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{2E62416A-70F5-4B75-9695-DAEC1D6A1865}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{2E62416A-70F5-4B75-9695-DAEC1D6A1865}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="1NF" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="81">
   <si>
     <t>ORDER_NUMBER</t>
   </si>
@@ -271,6 +272,12 @@
   </si>
   <si>
     <t>DeNormalised Sales Order Dataset</t>
+  </si>
+  <si>
+    <t>1st - Normal Form - Each column should have only values (Ensures atomicity)</t>
+  </si>
+  <si>
+    <t>now each columns contains only one values so this dataset is in 1st normal form</t>
   </si>
 </sst>
 </file>
@@ -332,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -348,6 +355,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,18 +675,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F229B0AA-798E-407C-95CD-F897669C1E8A}">
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView zoomScale="102" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:V9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -740,7 +751,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>10101</v>
       </c>
@@ -803,7 +814,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>10102</v>
       </c>
@@ -864,7 +875,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>10103</v>
       </c>
@@ -925,7 +936,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>10104</v>
       </c>
@@ -988,7 +999,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>10105</v>
       </c>
@@ -1049,7 +1060,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>10106</v>
       </c>
@@ -1110,7 +1121,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>75</v>
       </c>
@@ -1124,4 +1135,561 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDB2F79D-7E00-430A-8062-6E2F6B550BA7}">
+  <dimension ref="A2:U12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="7" max="7" width="27.77734375" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" customWidth="1"/>
+    <col min="12" max="12" width="25" customWidth="1"/>
+    <col min="13" max="13" width="22.33203125" customWidth="1"/>
+    <col min="14" max="14" width="14" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" customWidth="1"/>
+    <col min="20" max="20" width="12.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>10101</v>
+      </c>
+      <c r="B4" s="2">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2">
+        <v>202</v>
+      </c>
+      <c r="D4" s="2">
+        <v>6060</v>
+      </c>
+      <c r="E4" s="3">
+        <v>37704</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="2">
+        <v>200</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="2">
+        <v>2125357818</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" s="2">
+        <v>10022</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>10102</v>
+      </c>
+      <c r="B5" s="2">
+        <v>34</v>
+      </c>
+      <c r="C5" s="2">
+        <v>550</v>
+      </c>
+      <c r="D5" s="2">
+        <v>18700</v>
+      </c>
+      <c r="E5" s="3">
+        <v>37807</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="2">
+        <v>500</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" s="2">
+        <v>2123356666</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2">
+        <v>51100</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>10103</v>
+      </c>
+      <c r="B6" s="2">
+        <v>41</v>
+      </c>
+      <c r="C6" s="2">
+        <v>420</v>
+      </c>
+      <c r="D6" s="2">
+        <v>17220</v>
+      </c>
+      <c r="E6" s="3">
+        <v>37628</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="2">
+        <v>400</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="2">
+        <v>2121257800</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2">
+        <v>75508</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>10104</v>
+      </c>
+      <c r="B7" s="2">
+        <v>45</v>
+      </c>
+      <c r="C7" s="2">
+        <v>780</v>
+      </c>
+      <c r="D7" s="2">
+        <v>35100</v>
+      </c>
+      <c r="E7" s="3">
+        <v>37858</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" s="2">
+        <v>800</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K7" s="2">
+        <v>6265557265</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="P7" s="2">
+        <v>90003</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>10105</v>
+      </c>
+      <c r="B8" s="2">
+        <v>49</v>
+      </c>
+      <c r="C8" s="2">
+        <v>850</v>
+      </c>
+      <c r="D8" s="2">
+        <v>41650</v>
+      </c>
+      <c r="E8" s="3">
+        <v>37904</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" s="2">
+        <v>900</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K8" s="2">
+        <v>6505551386</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>10106</v>
+      </c>
+      <c r="B9" s="2">
+        <v>4</v>
+      </c>
+      <c r="C9" s="4">
+        <v>780</v>
+      </c>
+      <c r="D9" s="2">
+        <v>6520</v>
+      </c>
+      <c r="E9" s="3">
+        <v>38479</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I9" s="4">
+        <v>800</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K9" s="2">
+        <v>6577771000</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2">
+        <v>75016</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>10106</v>
+      </c>
+      <c r="B10" s="2">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>850</v>
+      </c>
+      <c r="D10" s="2">
+        <v>6520</v>
+      </c>
+      <c r="E10" s="3">
+        <v>38480</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10">
+        <v>900</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K10" s="2">
+        <v>6577771000</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P10" s="2">
+        <v>75016</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:U2"/>
+    <mergeCell ref="A12:XFD12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>